<commit_message>
performance evaluation duration of layout phase
</commit_message>
<xml_diff>
--- a/performanceAnalysis.xlsx
+++ b/performanceAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dev\studium\baArbeit\3DmultilayerGraphThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2BE270-FC32-438D-8BEA-9E112AEC9462}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34119684-07A4-47FE-B113-D56B2AFDF73B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17352" yWindow="0" windowWidth="23928" windowHeight="16680" tabRatio="190" xr2:uid="{14808D9F-CF4E-4A30-AF2E-ECFBBD287A6D}"/>
+    <workbookView xWindow="22840" yWindow="-2000" windowWidth="25787" windowHeight="13987" tabRatio="190" xr2:uid="{14808D9F-CF4E-4A30-AF2E-ECFBBD287A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Performance Analyse</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Exploration avg FPS</t>
+  </si>
+  <si>
+    <t>Layout Duration (s)</t>
   </si>
 </sst>
 </file>
@@ -107,8 +110,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -426,28 +432,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11AE7E2A-825D-4F0F-BA2B-828221400392}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -461,13 +469,16 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>310</v>
       </c>
@@ -481,13 +492,16 @@
         <v>40</v>
       </c>
       <c r="F5">
-        <v>90</v>
+        <v>5</v>
       </c>
       <c r="G5">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>730</v>
       </c>
@@ -501,13 +515,16 @@
         <v>30</v>
       </c>
       <c r="F6">
+        <v>7.5</v>
+      </c>
+      <c r="G6">
         <v>70</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1100</v>
       </c>
@@ -521,13 +538,16 @@
         <v>20</v>
       </c>
       <c r="F7">
+        <v>9.5</v>
+      </c>
+      <c r="G7">
         <v>55</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1560</v>
       </c>
@@ -541,13 +561,16 @@
         <v>20</v>
       </c>
       <c r="F8">
+        <v>10.5</v>
+      </c>
+      <c r="G8">
         <v>40</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>2343</v>
       </c>
@@ -561,13 +584,16 @@
         <v>10</v>
       </c>
       <c r="F9">
+        <v>15</v>
+      </c>
+      <c r="G9">
         <v>30</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>774</v>
       </c>
@@ -581,16 +607,19 @@
         <v>20</v>
       </c>
       <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
         <v>60</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>70</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>774</v>
       </c>
@@ -604,16 +633,19 @@
         <v>20</v>
       </c>
       <c r="F12">
+        <v>15</v>
+      </c>
+      <c r="G12">
         <v>55</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>70</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>774</v>
       </c>
@@ -627,16 +659,19 @@
         <v>10</v>
       </c>
       <c r="F13">
+        <v>27</v>
+      </c>
+      <c r="G13">
         <v>40</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>60</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>1560</v>
       </c>
@@ -650,13 +685,16 @@
         <v>5</v>
       </c>
       <c r="F14">
+        <v>30</v>
+      </c>
+      <c r="G14">
         <v>25</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>1020</v>
       </c>
@@ -670,10 +708,23 @@
         <v>10</v>
       </c>
       <c r="F15">
+        <v>20</v>
+      </c>
+      <c r="G15">
         <v>40</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F26">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>